<commit_message>
Ajuste nos dados do resumo
</commit_message>
<xml_diff>
--- a/back-dashboards-pyhton/oee.xlsx
+++ b/back-dashboards-pyhton/oee.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dashboards_python_html\dashboards-python-png\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dashboards_python\back-dashboards-pyhton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68D625D-89E3-4077-BEE4-E704BFEEA36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CBAA84-664B-4302-ABB0-4049DFDB7B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CF5629E2-5761-4C17-B986-64CC32C564C7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>linha</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>oee</t>
+  </si>
+  <si>
+    <t>Linha 2</t>
   </si>
 </sst>
 </file>
@@ -439,7 +442,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,7 +500,7 @@
         <v>45690</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>0.74539999999999995</v>
@@ -537,7 +540,7 @@
         <v>45751</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>0.75380000000000003</v>
@@ -577,7 +580,7 @@
         <v>45814</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>0.72650000000000003</v>
@@ -617,7 +620,7 @@
         <v>45877</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>0.98150000000000004</v>
@@ -657,7 +660,7 @@
         <v>45940</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>0.9728</v>
@@ -697,7 +700,7 @@
         <v>46003</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>0.98160000000000003</v>

</xml_diff>

<commit_message>
Implementação com o Dash
</commit_message>
<xml_diff>
--- a/back-dashboards-pyhton/oee.xlsx
+++ b/back-dashboards-pyhton/oee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dashboards_python\back-dashboards-pyhton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CBAA84-664B-4302-ABB0-4049DFDB7B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1B83C4-D974-4983-A10A-663C0ED0F306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CF5629E2-5761-4C17-B986-64CC32C564C7}"/>
   </bookViews>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A73F1879-BCB1-4262-BC3B-DF5969C7A128}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.93810000000000004</v>
+        <v>5.9381000000000004</v>
       </c>
       <c r="D2">
         <v>1.0059</v>
@@ -592,7 +592,7 @@
         <v>0.98839999999999995</v>
       </c>
       <c r="F7">
-        <v>0.66520000000000001</v>
+        <v>8.6652000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Conclusão de testes com dash
</commit_message>
<xml_diff>
--- a/back-dashboards-pyhton/oee.xlsx
+++ b/back-dashboards-pyhton/oee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dashboards_python\back-dashboards-pyhton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1B83C4-D974-4983-A10A-663C0ED0F306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C3C9A8-5D26-4EA4-A6C9-19C12EF9B018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CF5629E2-5761-4C17-B986-64CC32C564C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CF5629E2-5761-4C17-B986-64CC32C564C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>